<commit_message>
updated api model with state
</commit_message>
<xml_diff>
--- a/documentation/api_data_model.xlsx
+++ b/documentation/api_data_model.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>site_id</t>
   </si>
@@ -154,6 +154,30 @@
   </si>
   <si>
     <t>-117.0743278</t>
+  </si>
+  <si>
+    <t>site_name</t>
+  </si>
+  <si>
+    <t>name of the measurement site</t>
+  </si>
+  <si>
+    <t>state_id</t>
+  </si>
+  <si>
+    <t>state_name</t>
+  </si>
+  <si>
+    <t>state code</t>
+  </si>
+  <si>
+    <t>state name</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>California</t>
   </si>
 </sst>
 </file>
@@ -223,8 +247,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -250,15 +278,19 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,11 +620,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -641,51 +671,49 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
+      <c r="B3" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
+      <c r="B4" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
+      <c r="B5" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -693,16 +721,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -710,16 +738,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -727,16 +755,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -744,50 +772,50 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="120">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -795,32 +823,83 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="120">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>